<commit_message>
rob fixed and edits
</commit_message>
<xml_diff>
--- a/data/LSR2_robptsd_260124.xlsx
+++ b/data/LSR2_robptsd_260124.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Desktop\Github rep\LSR2_exercise_H\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/FS/HomeDrives/vc18e501/ESM/GALENOS - WP2/WP2/LSR2/LSR2_exercise_H/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF4777F-5BE5-4D72-941A-00BFAF317B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{038D7716-8D5C-9943-9EBD-51496C48F55B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{ADD00791-5F93-4E3A-AEAD-3C2028A1734B}"/>
+    <workbookView xWindow="4520" yWindow="500" windowWidth="23260" windowHeight="12460" xr2:uid="{ADD00791-5F93-4E3A-AEAD-3C2028A1734B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="19">
   <si>
     <t xml:space="preserve">Bryant2023 </t>
   </si>
@@ -93,9 +93,6 @@
   </si>
   <si>
     <t>Powers2015</t>
-  </si>
-  <si>
-    <t>Weight</t>
   </si>
 </sst>
 </file>
@@ -447,21 +444,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4D8EA4-06A4-47E4-B611-34C8982FC9C9}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.77734375" customWidth="1"/>
+    <col min="1" max="1" width="22.83203125" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="5" max="5" width="23.6640625" customWidth="1"/>
-    <col min="7" max="7" width="33.109375" customWidth="1"/>
+    <col min="7" max="7" width="33.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -483,11 +480,8 @@
       <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -509,11 +503,8 @@
       <c r="G2" t="s">
         <v>16</v>
       </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -535,11 +526,8 @@
       <c r="G3" t="s">
         <v>14</v>
       </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -561,11 +549,8 @@
       <c r="G4" t="s">
         <v>15</v>
       </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -587,11 +572,8 @@
       <c r="G5" t="s">
         <v>15</v>
       </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -613,11 +595,8 @@
       <c r="G6" t="s">
         <v>15</v>
       </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -639,11 +618,8 @@
       <c r="G7" t="s">
         <v>16</v>
       </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -665,11 +641,8 @@
       <c r="G8" t="s">
         <v>15</v>
       </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -691,11 +664,8 @@
       <c r="G9" t="s">
         <v>15</v>
       </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -716,9 +686,6 @@
       </c>
       <c r="G10" t="s">
         <v>16</v>
-      </c>
-      <c r="H10">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>